<commit_message>
Updated to allow for loading of data manually to project.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/aaron_hubbart_uipath_com/Documents/Documents/Documents/Product/Comms Mining/CommunicationsMiningDispatcherDirectToApi/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/aaron_hubbart_uipath_com/Documents/Documents/UiPath/Automation Sandbox/###GitHub/CommsMining/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{9A54EA7A-6B4F-43F4-93DE-5867E446C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9F450B2-2D9F-4560-AEBB-442CD337F488}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{9A54EA7A-6B4F-43F4-93DE-5867E446C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F23D299-E09D-401E-8B6B-64029FD704EA}"/>
   <bookViews>
-    <workbookView xWindow="-38940" yWindow="32400" windowWidth="38610" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38235" yWindow="32835" windowWidth="19365" windowHeight="20985" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -292,28 +292,37 @@
     <t>Folder name for asset containing the api token</t>
   </si>
   <si>
-    <t>CM Cross Org Test</t>
-  </si>
-  <si>
     <t>CM Token</t>
   </si>
   <si>
+    <t>check-dev-endpoint</t>
+  </si>
+  <si>
+    <t>OrchestratorFolderNameForQueue</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>CommunicationsMiningSourceName</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>Potential Case Finder Queue</t>
+  </si>
+  <si>
+    <t>The name of your source (should not include the project name)</t>
+  </si>
+  <si>
     <t>customer-services-inquiries</t>
   </si>
   <si>
+    <t>Inquiries</t>
+  </si>
+  <si>
     <t>Customer-Service</t>
-  </si>
-  <si>
-    <t>check-dev-endpoint</t>
-  </si>
-  <si>
-    <t>OrchestratorFolderNameForQueue</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>CM Test</t>
   </si>
 </sst>
 </file>
@@ -717,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -781,85 +790,95 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="B4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="b">
-        <f>FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <f>FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>80</v>
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>83</v>
+      <c r="C8" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>84</v>
+      <c r="C9" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1842,6 +1861,7 @@
     <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3125,7 +3145,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3180,7 +3200,7 @@
         <v>76</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
         <v>77</v>
@@ -3194,7 +3214,7 @@
         <v>78</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>79</v>

</xml_diff>